<commit_message>
changes to posfun and likelihoods
</commit_message>
<xml_diff>
--- a/xls/selectivity_scn.xlsx
+++ b/xls/selectivity_scn.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="-36020" yWindow="400" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -316,37 +316,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.0415481561997862</c:v>
+                  <c:v>0.0779352897004136</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0963228890285261</c:v>
+                  <c:v>0.165278460933939</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.207785014849124</c:v>
+                  <c:v>0.326140960149935</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.392628388461857</c:v>
+                  <c:v>0.563737831902844</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.615209947806279</c:v>
+                  <c:v>0.808022016566819</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.799354048973471</c:v>
+                  <c:v>0.960380616118389</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.909782877763076</c:v>
+                  <c:v>0.999876422111077</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.963481363205534</c:v>
+                  <c:v>0.96862628154551</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.986674491260958</c:v>
+                  <c:v>0.907384156934271</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.995907214052171</c:v>
+                  <c:v>0.837800338830846</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.999181829803003</c:v>
+                  <c:v>0.768901207283371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -405,37 +405,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.143234754423519</c:v>
+                  <c:v>0.235064663905296</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.291607482326815</c:v>
+                  <c:v>0.437765937224773</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.503969300008427</c:v>
+                  <c:v>0.692072744230843</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.715948802390102</c:v>
+                  <c:v>0.899360879923221</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.863405906062069</c:v>
+                  <c:v>0.992136443668782</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.941918706780358</c:v>
+                  <c:v>0.990088853980826</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.977604743980559</c:v>
+                  <c:v>0.940001207056023</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.992388624608872</c:v>
+                  <c:v>0.87287338200443</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.99800284029573</c:v>
+                  <c:v>0.802981632892002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.999772660127269</c:v>
+                  <c:v>0.735833324306859</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99996094862293</c:v>
+                  <c:v>0.673233312648593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -450,11 +450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2125297928"/>
-        <c:axId val="2125294760"/>
+        <c:axId val="2071122984"/>
+        <c:axId val="2071118200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2125297928"/>
+        <c:axId val="2071122984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -464,12 +464,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125294760"/>
+        <c:crossAx val="2071118200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2125294760"/>
+        <c:axId val="2071118200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125297928"/>
+        <c:crossAx val="2071122984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -862,7 +862,7 @@
   <dimension ref="D1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -903,10 +903,10 @@
         <v>1E-3</v>
       </c>
       <c r="N3">
-        <v>1E-3</v>
+        <v>0.1</v>
       </c>
       <c r="O3">
-        <v>1E-3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="4:15">
@@ -933,12 +933,12 @@
         <v>1.1124109603910968E-2</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:O22" si="0">(1/(1-N$3))*((1-N$3)/N$3)^N$3*((EXP(N$2*N$3*(N$1-$L5)))/(1+EXP(N$2*(N$1-$L5))))</f>
-        <v>4.1548156199786183E-2</v>
+        <f t="shared" ref="N5:O15" si="0">(1/(1-N$3))*((1-N$3)/N$3)^N$3*((EXP(N$2*N$3*(N$1-$L5)))/(1+EXP(N$2*(N$1-$L5))))</f>
+        <v>7.7935289700413621E-2</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>0.14323475442351938</v>
+        <v>0.23506466390529571</v>
       </c>
     </row>
     <row r="6" spans="4:15">
@@ -954,16 +954,16 @@
         <v>2</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M22" si="2">(1/(1-M$3))*((1-M$3)/M$3)^M$3*((EXP(M$2*M$3*(M$1-$L6)))/(1+EXP(M$2*(M$1-$L6))))</f>
+        <f t="shared" ref="M6:M15" si="2">(1/(1-M$3))*((1-M$3)/M$3)^M$3*((EXP(M$2*M$3*(M$1-$L6)))/(1+EXP(M$2*(M$1-$L6))))</f>
         <v>2.6904819687189479E-2</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>9.6322889028526135E-2</v>
+        <v>0.16527846093393886</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>0.2916074823268151</v>
+        <v>0.4377659372247733</v>
       </c>
     </row>
     <row r="7" spans="4:15">
@@ -975,7 +975,7 @@
         <v>5.9343034025940078</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L22" si="3">L6+1</f>
+        <f t="shared" ref="L7:L15" si="3">L6+1</f>
         <v>3</v>
       </c>
       <c r="M7">
@@ -984,11 +984,11 @@
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>0.20778501484912382</v>
+        <v>0.32614096014993477</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>0.50396930000842732</v>
+        <v>0.69207274423084297</v>
       </c>
     </row>
     <row r="8" spans="4:15">
@@ -1009,11 +1009,11 @@
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>0.39262838846185716</v>
+        <v>0.5637378319028441</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>0.71594880239010217</v>
+        <v>0.89936087992322156</v>
       </c>
     </row>
     <row r="9" spans="4:15">
@@ -1034,11 +1034,11 @@
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>0.6152099478062788</v>
+        <v>0.80802201656681905</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>0.86340590606206924</v>
+        <v>0.9921364436687824</v>
       </c>
     </row>
     <row r="10" spans="4:15">
@@ -1059,11 +1059,11 @@
       </c>
       <c r="N10">
         <f t="shared" si="0"/>
-        <v>0.7993540489734714</v>
+        <v>0.96038061611838876</v>
       </c>
       <c r="O10">
         <f t="shared" si="0"/>
-        <v>0.94191870678035838</v>
+        <v>0.99008885398082591</v>
       </c>
     </row>
     <row r="11" spans="4:15">
@@ -1084,11 +1084,11 @@
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
-        <v>0.90978287776307598</v>
+        <v>0.99987642211107752</v>
       </c>
       <c r="O11">
         <f t="shared" si="0"/>
-        <v>0.97760474398055908</v>
+        <v>0.94000120705602286</v>
       </c>
     </row>
     <row r="12" spans="4:15">
@@ -1109,11 +1109,11 @@
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>0.96348136320553379</v>
+        <v>0.96862628154551011</v>
       </c>
       <c r="O12">
         <f t="shared" si="0"/>
-        <v>0.99238862460887156</v>
+        <v>0.8728733820044301</v>
       </c>
     </row>
     <row r="13" spans="4:15" ht="19">
@@ -1137,11 +1137,11 @@
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>0.98667449126095841</v>
+        <v>0.90738415693427077</v>
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>0.99800284029573039</v>
+        <v>0.80298163289200175</v>
       </c>
     </row>
     <row r="14" spans="4:15">
@@ -1162,11 +1162,11 @@
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>0.99590721405217142</v>
+        <v>0.8378003388308457</v>
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
-        <v>0.99977266012726917</v>
+        <v>0.7358333243068591</v>
       </c>
     </row>
     <row r="15" spans="4:15">
@@ -1180,11 +1180,11 @@
       </c>
       <c r="N15">
         <f t="shared" si="0"/>
-        <v>0.99918182980300352</v>
+        <v>0.76890120728337141</v>
       </c>
       <c r="O15">
         <f t="shared" si="0"/>
-        <v>0.99996094862292961</v>
+        <v>0.67323331264859265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
endo of day - low bias
</commit_message>
<xml_diff>
--- a/xls/selectivity_scn.xlsx
+++ b/xls/selectivity_scn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36020" yWindow="400" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-36020" yWindow="20" windowWidth="25600" windowHeight="16800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -862,7 +862,7 @@
   <dimension ref="D1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>